<commit_message>
add script to capture how many times a time series has changed its moving directions
</commit_message>
<xml_diff>
--- a/Noise Analysis/pandapas_noise.xlsx
+++ b/Noise Analysis/pandapas_noise.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuezheli/Desktop/Benchmarking_TSDiscretizations/Noise Analysis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7882AE81-12FF-2643-894A-03243C55DDE0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22320" windowHeight="13540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22320" windowHeight="13540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pandapas_DiscreeTest" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
     <sheet name="weighted confusion matrix" sheetId="3" r:id="rId3"/>
     <sheet name="AUROC" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -225,8 +231,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +254,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
@@ -324,11 +338,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -379,6 +395,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -703,19 +727,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -753,132 +777,132 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>0.5078125</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>0.40385748705279501</v>
       </c>
       <c r="F2" s="1">
         <v>0.01</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>0.5078125</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>0.402311087025914</v>
       </c>
       <c r="K2" s="1">
         <v>0.05</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="3">
         <v>0.5078125</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="3">
         <v>0.402217538507327</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="B3" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.1796875</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.490126244475381</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>0.1796875</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>0.49060730013612602</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="3">
         <v>0.1796875</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="3">
         <v>0.49050508006405802</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>3.90625E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>0.35808876978881499</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>3.90625E-2</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>0.42947738590009199</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="3">
         <v>3.90625E-2</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="3">
         <v>0.42941691589479097</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="B5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>3.90625E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.36314898412902002</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>3.90625E-2</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="4">
         <v>0.35806608039501903</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>3.90625E-2</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>0.35795762141058801</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -907,7 +931,7 @@
         <v>0.34758488783636698</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -936,7 +960,7 @@
         <v>0.40992973640761199</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -965,7 +989,7 @@
         <v>0.40992973640761199</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -994,7 +1018,7 @@
         <v>0.25999211139005801</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -1023,7 +1047,7 @@
         <v>0.38678766461062902</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1052,7 +1076,7 @@
         <v>0.43022553399387697</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +1105,7 @@
         <v>0.37789681953437099</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -1110,7 +1134,7 @@
         <v>0.238671842086424</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1139,7 +1163,7 @@
         <v>0.38804968273583401</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -1168,7 +1192,7 @@
         <v>0.39259767423522601</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -1197,7 +1221,7 @@
         <v>0.40148851931148299</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -1226,7 +1250,7 @@
         <v>0.381655532627729</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -1255,7 +1279,7 @@
         <v>0.26913805981738298</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -1284,7 +1308,7 @@
         <v>0.39605432620307202</v>
       </c>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -1313,7 +1337,7 @@
         <v>0.46642317932119098</v>
       </c>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -1342,7 +1366,7 @@
         <v>0.474336798639583</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -1371,7 +1395,7 @@
         <v>0.482651569588264</v>
       </c>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>25</v>
       </c>
@@ -1400,7 +1424,7 @@
         <v>0.40275053743668898</v>
       </c>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -1441,14 +1465,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
@@ -1458,27 +1482,27 @@
     <col min="7" max="7" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1504,7 +1528,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1530,7 +1554,7 @@
         <v>9.6385542168674704E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -1553,7 +1577,7 @@
         <v>0.14056224899598399</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -1576,7 +1600,7 @@
         <v>0.160642570281125</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>41</v>
       </c>
@@ -1599,7 +1623,7 @@
         <v>0.120481927710843</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1625,7 +1649,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0.01</v>
       </c>
@@ -1651,7 +1675,7 @@
         <v>6.82730923694779E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1674,7 +1698,7 @@
         <v>0.16465863453815299</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>40</v>
       </c>
@@ -1697,7 +1721,7 @@
         <v>0.184738955823293</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>41</v>
       </c>
@@ -1720,7 +1744,7 @@
         <v>9.6385542168674704E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1746,7 +1770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0.05</v>
       </c>
@@ -1772,7 +1796,7 @@
         <v>6.82730923694779E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -1795,7 +1819,7 @@
         <v>0.16465863453815299</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>40</v>
       </c>
@@ -1818,7 +1842,7 @@
         <v>0.184738955823293</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>41</v>
       </c>
@@ -1853,36 +1877,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1908,7 +1932,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1934,7 +1958,7 @@
         <v>0.28510057760101398</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -1957,7 +1981,7 @@
         <v>0.29663309082798001</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -1980,7 +2004,7 @@
         <v>5.73590267534205E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>41</v>
       </c>
@@ -2003,7 +2027,7 @@
         <v>3.1619930789681901E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2029,7 +2053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0.01</v>
       </c>
@@ -2055,7 +2079,7 @@
         <v>0.49435064774675003</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -2078,7 +2102,7 @@
         <v>0.29687060983380698</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>40</v>
       </c>
@@ -2101,7 +2125,7 @@
         <v>0.20219937749935499</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>41</v>
       </c>
@@ -2124,7 +2148,7 @@
         <v>0.28510057760101398</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2150,7 +2174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0.05</v>
       </c>
@@ -2176,7 +2200,7 @@
         <v>0.49435064774675003</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2199,7 +2223,7 @@
         <v>0.29687060983380698</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>40</v>
       </c>
@@ -2222,7 +2246,7 @@
         <v>0.20219937749935499</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>41</v>
       </c>
@@ -2257,14 +2281,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
@@ -2272,7 +2296,7 @@
     <col min="8" max="8" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -2298,7 +2322,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2324,7 +2348,7 @@
         <v>0.54947368429806998</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
@@ -2338,7 +2362,7 @@
         <v>0.65947368429263198</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>46</v>
       </c>
@@ -2352,7 +2376,7 @@
         <v>0.50087719322912305</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>47</v>
       </c>
@@ -2366,7 +2390,7 @@
         <v>0.55263157900000004</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>48</v>
       </c>
@@ -2380,7 +2404,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>49</v>
       </c>
@@ -2394,7 +2418,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>41</v>
       </c>
@@ -2408,7 +2432,7 @@
         <v>0.62315789494631602</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>50</v>
       </c>
@@ -2422,7 +2446,7 @@
         <v>0.45824561422912302</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>51</v>
       </c>
@@ -2436,7 +2460,7 @@
         <v>0.50087719322912305</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>40</v>
       </c>
@@ -2450,7 +2474,7 @@
         <v>0.597543859782807</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>39</v>
       </c>
@@ -2464,7 +2488,7 @@
         <v>0.54912280689456106</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>54</v>
       </c>
@@ -2472,7 +2496,7 @@
         <v>0.87891534403100502</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>55</v>
       </c>
@@ -2480,7 +2504,7 @@
         <v>0.80399999990000004</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>56</v>
       </c>
@@ -2488,7 +2512,7 @@
         <v>0.86203703708101798</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>57</v>
       </c>
@@ -2496,7 +2520,7 @@
         <v>0.86328703709101895</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>58</v>
       </c>
@@ -2504,7 +2528,7 @@
         <v>0.85119047601297604</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>59</v>
       </c>
@@ -2512,7 +2536,7 @@
         <v>0.83742857137095195</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>60</v>
       </c>
@@ -2520,7 +2544,7 @@
         <v>0.85285714269595303</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>61</v>
       </c>
@@ -2528,7 +2552,7 @@
         <v>0.82777777774555605</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>62</v>
       </c>
@@ -2536,7 +2560,7 @@
         <v>0.84333333314095205</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>63</v>
       </c>
@@ -2544,7 +2568,7 @@
         <v>0.88691919205792902</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>64</v>
       </c>
@@ -2552,7 +2576,7 @@
         <v>0.87814814803851904</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>65</v>
       </c>
@@ -2560,7 +2584,7 @@
         <v>0.85367063511999997</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2586,7 +2610,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0.01</v>
       </c>
@@ -2612,7 +2636,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>38</v>
       </c>
@@ -2626,7 +2650,7 @@
         <v>0.55894736847438597</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>46</v>
       </c>
@@ -2640,7 +2664,7 @@
         <v>0.50087719322912305</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>47</v>
       </c>
@@ -2654,7 +2678,7 @@
         <v>0.55263157900000004</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
         <v>48</v>
       </c>
@@ -2668,7 +2692,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="3:9">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>49</v>
       </c>
@@ -2682,7 +2706,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="3:9">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>41</v>
       </c>
@@ -2696,7 +2720,7 @@
         <v>0.62315789494631602</v>
       </c>
     </row>
-    <row r="35" spans="3:9">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>50</v>
       </c>
@@ -2710,7 +2734,7 @@
         <v>0.50842105288456096</v>
       </c>
     </row>
-    <row r="36" spans="3:9">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>51</v>
       </c>
@@ -2724,7 +2748,7 @@
         <v>0.50087719322912305</v>
       </c>
     </row>
-    <row r="37" spans="3:9">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>40</v>
       </c>
@@ -2738,7 +2762,7 @@
         <v>0.59543859677736799</v>
       </c>
     </row>
-    <row r="38" spans="3:9">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>39</v>
       </c>
@@ -2752,7 +2776,7 @@
         <v>0.57192982481543897</v>
       </c>
     </row>
-    <row r="39" spans="3:9">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>54</v>
       </c>
@@ -2760,7 +2784,7 @@
         <v>0.87891534403100502</v>
       </c>
     </row>
-    <row r="40" spans="3:9">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>55</v>
       </c>
@@ -2768,7 +2792,7 @@
         <v>0.80399999990000004</v>
       </c>
     </row>
-    <row r="41" spans="3:9">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>56</v>
       </c>
@@ -2776,7 +2800,7 @@
         <v>0.86203703708101798</v>
       </c>
     </row>
-    <row r="42" spans="3:9">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>57</v>
       </c>
@@ -2784,7 +2808,7 @@
         <v>0.86328703709101895</v>
       </c>
     </row>
-    <row r="43" spans="3:9">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
         <v>58</v>
       </c>
@@ -2792,7 +2816,7 @@
         <v>0.85119047601297604</v>
       </c>
     </row>
-    <row r="44" spans="3:9">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>59</v>
       </c>
@@ -2800,7 +2824,7 @@
         <v>0.84386904738297597</v>
       </c>
     </row>
-    <row r="45" spans="3:9">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>60</v>
       </c>
@@ -2808,7 +2832,7 @@
         <v>0.85285714269595303</v>
       </c>
     </row>
-    <row r="46" spans="3:9">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>61</v>
       </c>
@@ -2816,7 +2840,7 @@
         <v>0.84333333314095205</v>
       </c>
     </row>
-    <row r="47" spans="3:9">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
         <v>62</v>
       </c>
@@ -2824,7 +2848,7 @@
         <v>0.80733333330000001</v>
       </c>
     </row>
-    <row r="48" spans="3:9">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>63</v>
       </c>
@@ -2832,7 +2856,7 @@
         <v>0.86067195760391502</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
         <v>64</v>
       </c>
@@ -2840,7 +2864,7 @@
         <v>0.84263888888444505</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>65</v>
       </c>
@@ -2848,7 +2872,7 @@
         <v>0.87140740758148205</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -2874,7 +2898,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>0.05</v>
       </c>
@@ -2900,7 +2924,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
         <v>38</v>
       </c>
@@ -2914,7 +2938,7 @@
         <v>0.55894736847438597</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
         <v>46</v>
       </c>
@@ -2928,7 +2952,7 @@
         <v>0.50087719322912305</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
         <v>47</v>
       </c>
@@ -2942,7 +2966,7 @@
         <v>0.55263157900000004</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
         <v>48</v>
       </c>
@@ -2956,7 +2980,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
         <v>49</v>
       </c>
@@ -2970,7 +2994,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
         <v>41</v>
       </c>
@@ -2984,7 +3008,7 @@
         <v>0.62315789494631602</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
         <v>50</v>
       </c>
@@ -2998,7 +3022,7 @@
         <v>0.50842105288456096</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
         <v>51</v>
       </c>
@@ -3012,7 +3036,7 @@
         <v>0.50087719322912305</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
         <v>40</v>
       </c>
@@ -3026,7 +3050,7 @@
         <v>0.59543859677736799</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
         <v>39</v>
       </c>
@@ -3040,7 +3064,7 @@
         <v>0.57192982481543897</v>
       </c>
     </row>
-    <row r="65" spans="3:4">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>54</v>
       </c>
@@ -3048,7 +3072,7 @@
         <v>0.87891534403100502</v>
       </c>
     </row>
-    <row r="66" spans="3:4">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
         <v>55</v>
       </c>
@@ -3056,7 +3080,7 @@
         <v>0.80399999990000004</v>
       </c>
     </row>
-    <row r="67" spans="3:4">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
         <v>56</v>
       </c>
@@ -3064,7 +3088,7 @@
         <v>0.86203703708101798</v>
       </c>
     </row>
-    <row r="68" spans="3:4">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
         <v>57</v>
       </c>
@@ -3072,7 +3096,7 @@
         <v>0.86328703709101895</v>
       </c>
     </row>
-    <row r="69" spans="3:4">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
         <v>58</v>
       </c>
@@ -3080,7 +3104,7 @@
         <v>0.85119047601297604</v>
       </c>
     </row>
-    <row r="70" spans="3:4">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
         <v>59</v>
       </c>
@@ -3088,7 +3112,7 @@
         <v>0.84386904738297597</v>
       </c>
     </row>
-    <row r="71" spans="3:4">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
         <v>60</v>
       </c>
@@ -3096,7 +3120,7 @@
         <v>0.77833333324999998</v>
       </c>
     </row>
-    <row r="72" spans="3:4">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
         <v>61</v>
       </c>
@@ -3104,7 +3128,7 @@
         <v>0.84333333314095205</v>
       </c>
     </row>
-    <row r="73" spans="3:4">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
         <v>62</v>
       </c>
@@ -3112,7 +3136,7 @@
         <v>0.80733333330000001</v>
       </c>
     </row>
-    <row r="74" spans="3:4">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
         <v>63</v>
       </c>
@@ -3120,7 +3144,7 @@
         <v>0.86067195760391502</v>
       </c>
     </row>
-    <row r="75" spans="3:4">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>64</v>
       </c>
@@ -3128,7 +3152,7 @@
         <v>0.84263888888444505</v>
       </c>
     </row>
-    <row r="76" spans="3:4">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
add trend confusion matrix analysis
</commit_message>
<xml_diff>
--- a/Noise Analysis/pandapas_noise.xlsx
+++ b/Noise Analysis/pandapas_noise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuezheli/Desktop/Benchmarking_TSDiscretizations/Noise Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7882AE81-12FF-2643-894A-03243C55DDE0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800333D2-C8C2-4241-988E-80DFF13B8F28}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22320" windowHeight="13540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="540" windowWidth="22320" windowHeight="13540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pandapas_DiscreeTest" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="78">
   <si>
     <t>discretization</t>
   </si>
@@ -226,13 +226,49 @@
   </si>
   <si>
     <t>q5</t>
+  </si>
+  <si>
+    <t>accurary</t>
+  </si>
+  <si>
+    <t>confusion matrix based on whether original data and discretized data show the same increase/ decrease between two specific time steps</t>
+  </si>
+  <si>
+    <t>TP: correctly identified local maxima (infliction points that  signals the trend from increasing to decreasing)</t>
+  </si>
+  <si>
+    <t>TN: correctly identified local minima (infliction points that signals the trend from decreasing to increasing)</t>
+  </si>
+  <si>
+    <t>FP: misidentified local maxima (local maxima that appear in discretized data but not in original data) or missed local minima (local minima in original data but not in discretized data)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FN: misidentified local minima (local minima that appear in discretized data but not in original data) or missed local maxima ( local maxima in the original data but not in discretized data) </t>
+  </si>
+  <si>
+    <t>confusion matrix based on infliction points</t>
+  </si>
+  <si>
+    <t>positive predicted value (ppv)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivity </t>
+  </si>
+  <si>
+    <t>specificity</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>f1 score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,8 +303,24 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,13 +333,105 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -338,13 +482,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -395,6 +557,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF95FF3A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -730,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:N5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,241 +948,241 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.5078125</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.40385748705279501</v>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="D2">
+        <v>0.23873300813093501</v>
       </c>
       <c r="F2" s="1">
         <v>0.01</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.5078125</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.402311087025914</v>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="I2">
+        <v>0.23871192820720299</v>
       </c>
       <c r="K2" s="1">
         <v>0.05</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0.5078125</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.402217538507327</v>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="N2">
+        <v>0.238671842086424</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.1796875</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.490126244475381</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.1796875</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.49060730013612602</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0.1796875</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0.49050508006405802</v>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="D3">
+        <v>0.26010850583974998</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="I3">
+        <v>0.26008928909767798</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="N3">
+        <v>0.25999211139005801</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="D4">
+        <v>0.26926831830606002</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="I4">
+        <v>0.26924851390556997</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="N4">
+        <v>0.26913805981738298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="D5">
+        <v>0.28183198707368701</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="I5">
+        <v>0.347635196125404</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="N5">
+        <v>0.34758488783636698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C6" s="4">
         <v>3.90625E-2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D6" s="4">
         <v>0.35808876978881499</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="4">
         <v>3.90625E-2</v>
       </c>
-      <c r="I4" s="3">
-        <v>0.42947738590009199</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="3">
+      <c r="I6" s="4">
+        <v>0.35806608039501903</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="4">
         <v>3.90625E-2</v>
       </c>
-      <c r="N4" s="3">
-        <v>0.42941691589479097</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="N6" s="4">
+        <v>0.35795762141058801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C7" s="3">
         <v>3.90625E-2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D7" s="3">
         <v>0.36314898412902002</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="4">
-        <v>3.90625E-2</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0.35806608039501903</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="4">
-        <v>3.90625E-2</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0.35795762141058801</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="D6">
-        <v>0.28183198707368701</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="I6">
-        <v>0.347635196125404</v>
-      </c>
-      <c r="L6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N6">
-        <v>0.34758488783636698</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="D7">
-        <v>0.41001496255370901</v>
-      </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H7">
         <v>3.90625E-3</v>
       </c>
       <c r="I7">
-        <v>0.40999020641291301</v>
+        <v>0.37796554549689199</v>
       </c>
       <c r="L7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="M7">
         <v>3.90625E-3</v>
       </c>
       <c r="N7">
-        <v>0.40992973640761199</v>
+        <v>0.37789681953437099</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>3.90625E-3</v>
       </c>
       <c r="D8">
-        <v>0.41001496255370901</v>
+        <v>0.37908684599912201</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>3.90625E-3</v>
       </c>
       <c r="I8">
-        <v>0.40999020641291301</v>
+        <v>0.38175954481019803</v>
       </c>
       <c r="L8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="M8">
         <v>3.90625E-3</v>
       </c>
       <c r="N8">
-        <v>0.40992973640761199</v>
+        <v>0.381655532627729</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>3.90625E-3</v>
       </c>
       <c r="D9">
-        <v>0.26010850583974998</v>
+        <v>0.38194597578985101</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H9">
         <v>3.90625E-3</v>
       </c>
       <c r="I9">
-        <v>0.26008928909767798</v>
+        <v>0.386697000923377</v>
       </c>
       <c r="L9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="M9">
         <v>3.90625E-3</v>
       </c>
       <c r="N9">
-        <v>0.25999211139005801</v>
+        <v>0.38661683640634398</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1049,411 +1216,414 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>3.90625E-3</v>
       </c>
       <c r="D11">
-        <v>0.42805581126203801</v>
+        <v>0.38813148192945601</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H11">
         <v>3.90625E-3</v>
       </c>
       <c r="I11">
-        <v>0.430376555162296</v>
+        <v>0.38810544365740302</v>
       </c>
       <c r="L11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M11">
         <v>3.90625E-3</v>
       </c>
       <c r="N11">
-        <v>0.43022553399387697</v>
+        <v>0.38804968273583401</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>3.90625E-3</v>
       </c>
       <c r="D12">
-        <v>0.38194597578985101</v>
+        <v>0.38836153379848998</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H12">
         <v>3.90625E-3</v>
       </c>
       <c r="I12">
-        <v>0.37796554549689199</v>
+        <v>0.39266640019774701</v>
       </c>
       <c r="L12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M12">
         <v>3.90625E-3</v>
       </c>
       <c r="N12">
-        <v>0.37789681953437099</v>
+        <v>0.39259767423522601</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>3.90625E-3</v>
       </c>
       <c r="D13">
-        <v>0.23873300813093501</v>
+        <v>0.39618000354410299</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H13">
         <v>3.90625E-3</v>
       </c>
       <c r="I13">
-        <v>0.23871192820720299</v>
+        <v>0.39615227148666698</v>
       </c>
       <c r="L13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M13">
         <v>3.90625E-3</v>
       </c>
       <c r="N13">
-        <v>0.238671842086424</v>
+        <v>0.39605432620307202</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>3.90625E-3</v>
       </c>
       <c r="D14">
-        <v>0.38813148192945601</v>
+        <v>0.39664683049070598</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H14">
         <v>3.90625E-3</v>
       </c>
       <c r="I14">
-        <v>0.38810544365740302</v>
+        <v>0.40156877150664599</v>
       </c>
       <c r="L14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M14">
         <v>3.90625E-3</v>
       </c>
       <c r="N14">
-        <v>0.38804968273583401</v>
+        <v>0.40148851931148299</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>3.90625E-3</v>
       </c>
       <c r="D15">
-        <v>0.39664683049070598</v>
-      </c>
-      <c r="G15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="I15">
-        <v>0.39266640019774701</v>
-      </c>
-      <c r="L15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N15">
-        <v>0.39259767423522601</v>
+        <v>0.40172910776759502</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.5078125</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.402311087025914</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0.5078125</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0.402217538507327</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>3.90625E-3</v>
       </c>
       <c r="D16">
-        <v>0.40172910776759502</v>
+        <v>0.40283233663031098</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H16">
         <v>3.90625E-3</v>
       </c>
       <c r="I16">
-        <v>0.40156877150664599</v>
+        <v>0.40280629835825799</v>
       </c>
       <c r="L16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M16">
         <v>3.90625E-3</v>
       </c>
       <c r="N16">
-        <v>0.40148851931148299</v>
+        <v>0.40275053743668898</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="D17">
-        <v>0.37908684599912201</v>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.5078125</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.40385748705279501</v>
       </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H17">
         <v>3.90625E-3</v>
       </c>
       <c r="I17">
-        <v>0.38175954481019803</v>
+        <v>0.40999020641291301</v>
       </c>
       <c r="L17" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="M17">
         <v>3.90625E-3</v>
       </c>
       <c r="N17">
-        <v>0.381655532627729</v>
+        <v>0.40992973640761199</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>3.90625E-3</v>
       </c>
       <c r="D18">
-        <v>0.26926831830606002</v>
+        <v>0.41001496255370901</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H18">
         <v>3.90625E-3</v>
       </c>
       <c r="I18">
-        <v>0.26924851390556997</v>
+        <v>0.40999020641291301</v>
       </c>
       <c r="L18" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="M18">
         <v>3.90625E-3</v>
       </c>
       <c r="N18">
-        <v>0.26913805981738298</v>
+        <v>0.40992973640761199</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>3.90625E-3</v>
       </c>
       <c r="D19">
-        <v>0.39618000354410299</v>
-      </c>
-      <c r="G19" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="I19">
-        <v>0.39615227148666698</v>
-      </c>
-      <c r="L19" t="s">
-        <v>21</v>
-      </c>
-      <c r="M19">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N19">
-        <v>0.39605432620307202</v>
+        <v>0.41001496255370901</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3.90625E-2</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.42947738590009199</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3.90625E-2</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0.42941691589479097</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>3.90625E-3</v>
       </c>
       <c r="D20">
-        <v>0.46644480873385802</v>
+        <v>0.42805581126203801</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H20">
         <v>3.90625E-3</v>
       </c>
       <c r="I20">
-        <v>0.46642404178890401</v>
+        <v>0.430376555162296</v>
       </c>
       <c r="L20" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="M20">
         <v>3.90625E-3</v>
       </c>
       <c r="N20">
-        <v>0.46642317932119098</v>
+        <v>0.43022553399387697</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>3.90625E-3</v>
       </c>
       <c r="D21">
-        <v>0.47435766859135098</v>
+        <v>0.46644480873385802</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H21">
         <v>3.90625E-3</v>
       </c>
       <c r="I21">
-        <v>0.474337153099256</v>
+        <v>0.46642404178890401</v>
       </c>
       <c r="L21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M21">
         <v>3.90625E-3</v>
       </c>
       <c r="N21">
-        <v>0.474336798639583</v>
+        <v>0.46642317932119098</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>3.90625E-3</v>
       </c>
       <c r="D22">
-        <v>0.48266665978916401</v>
+        <v>0.47435766859135098</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H22">
         <v>3.90625E-3</v>
       </c>
       <c r="I22">
-        <v>0.482645104422806</v>
+        <v>0.474337153099256</v>
       </c>
       <c r="L22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M22">
         <v>3.90625E-3</v>
       </c>
       <c r="N22">
-        <v>0.482651569588264</v>
+        <v>0.474336798639583</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>3.90625E-3</v>
       </c>
       <c r="D23">
-        <v>0.40283233663031098</v>
+        <v>0.48266665978916401</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23">
         <v>3.90625E-3</v>
       </c>
       <c r="I23">
-        <v>0.40280629835825799</v>
+        <v>0.482645104422806</v>
       </c>
       <c r="L23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M23">
         <v>3.90625E-3</v>
       </c>
       <c r="N23">
-        <v>0.40275053743668898</v>
+        <v>0.482651569588264</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="D24">
-        <v>0.38836153379848998</v>
-      </c>
-      <c r="G24" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="I24">
-        <v>0.386697000923377</v>
-      </c>
-      <c r="L24" t="s">
-        <v>26</v>
-      </c>
-      <c r="M24">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N24">
-        <v>0.38661683640634398</v>
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.1796875</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.490126244475381</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.1796875</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.49060730013612602</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0.1796875</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0.49050508006405802</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="L2:N24">
+    <sortCondition ref="N2:N24"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1466,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1479,390 +1649,1689 @@
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
     <col min="6" max="6" width="21.1640625" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="I6" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>24</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>225</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>244</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>19</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>8.9552238805970102E-2</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>9.6385542168674704E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="I7" s="6">
+        <v>8.3984375E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>35</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>214</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>240</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>23</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <v>0.12727272727272701</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="6">
         <v>0.14056224899598399</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="I8" s="6">
+        <v>0.11328125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>40</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>209</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>228</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>35</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>0.14925373134328401</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <v>0.160642570281125</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="I9" s="6">
+        <v>0.146484375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>30</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>219</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>202</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>61</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <v>0.12931034482758599</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
         <v>0.120481927710843</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="I10" s="6">
+        <v>0.177734375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="6">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6">
+        <v>222</v>
+      </c>
+      <c r="E11" s="6">
+        <v>244</v>
+      </c>
+      <c r="F11" s="6">
+        <v>19</v>
+      </c>
+      <c r="G11" s="6">
+        <v>9.9630996309963096E-2</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.108433734939759</v>
+      </c>
+      <c r="I11" s="6">
+        <v>8.984375E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="6">
+        <v>17</v>
+      </c>
+      <c r="D12" s="6">
+        <v>232</v>
+      </c>
+      <c r="E12" s="6">
+        <v>245</v>
+      </c>
+      <c r="F12" s="6">
+        <v>18</v>
+      </c>
+      <c r="G12" s="6">
+        <v>6.4885496183206104E-2</v>
+      </c>
+      <c r="H12" s="6">
+        <v>6.82730923694779E-2</v>
+      </c>
+      <c r="I12" s="6">
+        <v>6.8359375E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="I14" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
         <v>0.01</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C14">
+      <c r="C15" s="6">
         <v>17</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="6">
         <v>232</v>
       </c>
-      <c r="E14">
+      <c r="E15" s="6">
         <v>250</v>
       </c>
-      <c r="F14">
+      <c r="F15" s="6">
         <v>13</v>
       </c>
-      <c r="G14">
+      <c r="G15" s="6">
         <v>6.3670411985018702E-2</v>
       </c>
-      <c r="H14">
+      <c r="H15" s="6">
         <v>6.82730923694779E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="I15" s="6">
+        <v>5.859375E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="6">
         <v>41</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="6">
         <v>208</v>
       </c>
-      <c r="E15">
+      <c r="E16" s="6">
         <v>238</v>
       </c>
-      <c r="F15">
+      <c r="F16" s="6">
         <v>25</v>
       </c>
-      <c r="G15">
+      <c r="G16" s="6">
         <v>0.14695340501792101</v>
       </c>
-      <c r="H15">
+      <c r="H16" s="6">
         <v>0.16465863453815299</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="I16" s="6">
+        <v>0.12890625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="6">
         <v>46</v>
       </c>
-      <c r="D16">
+      <c r="D17" s="6">
         <v>203</v>
       </c>
-      <c r="E16">
+      <c r="E17" s="6">
         <v>216</v>
       </c>
-      <c r="F16">
+      <c r="F17" s="6">
         <v>47</v>
       </c>
-      <c r="G16">
+      <c r="G17" s="6">
         <v>0.17557251908396901</v>
       </c>
-      <c r="H16">
+      <c r="H17" s="6">
         <v>0.184738955823293</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="I17" s="6">
+        <v>0.181640625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="6">
         <v>24</v>
       </c>
-      <c r="D17">
+      <c r="D18" s="6">
         <v>225</v>
       </c>
-      <c r="E17">
+      <c r="E18" s="6">
         <v>244</v>
       </c>
-      <c r="F17">
+      <c r="F18" s="6">
         <v>19</v>
       </c>
-      <c r="G17">
+      <c r="G18" s="6">
         <v>8.9552238805970102E-2</v>
       </c>
-      <c r="H17">
+      <c r="H18" s="6">
         <v>9.6385542168674704E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="I18" s="6">
+        <v>8.3984375E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="6">
+        <v>27</v>
+      </c>
+      <c r="D19" s="6">
+        <v>222</v>
+      </c>
+      <c r="E19" s="6">
+        <v>244</v>
+      </c>
+      <c r="F19" s="6">
+        <v>19</v>
+      </c>
+      <c r="G19" s="6">
+        <v>9.9630996309963096E-2</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.108433734939759</v>
+      </c>
+      <c r="I19" s="6">
+        <v>8.984375E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="6">
+        <v>17</v>
+      </c>
+      <c r="D20" s="6">
+        <v>232</v>
+      </c>
+      <c r="E20" s="6">
+        <v>245</v>
+      </c>
+      <c r="F20" s="6">
+        <v>18</v>
+      </c>
+      <c r="G20" s="6">
+        <v>6.4885496183206104E-2</v>
+      </c>
+      <c r="H20" s="6">
+        <v>6.82730923694779E-2</v>
+      </c>
+      <c r="I20" s="6">
+        <v>6.8359375E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H22" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="I22" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <v>0.05</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C21">
+      <c r="C23" s="6">
         <v>17</v>
       </c>
-      <c r="D21">
+      <c r="D23" s="6">
         <v>232</v>
       </c>
-      <c r="E21">
+      <c r="E23" s="6">
         <v>250</v>
       </c>
-      <c r="F21">
+      <c r="F23" s="6">
         <v>13</v>
       </c>
-      <c r="G21">
+      <c r="G23" s="6">
         <v>6.3670411985018702E-2</v>
       </c>
-      <c r="H21">
+      <c r="H23" s="6">
         <v>6.82730923694779E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+      <c r="I23" s="6">
+        <v>5.859375E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C22">
+      <c r="C24" s="6">
         <v>41</v>
       </c>
-      <c r="D22">
+      <c r="D24" s="6">
         <v>208</v>
       </c>
-      <c r="E22">
+      <c r="E24" s="6">
         <v>238</v>
       </c>
-      <c r="F22">
+      <c r="F24" s="6">
         <v>25</v>
       </c>
-      <c r="G22">
+      <c r="G24" s="6">
         <v>0.14695340501792101</v>
       </c>
-      <c r="H22">
+      <c r="H24" s="6">
         <v>0.16465863453815299</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="I24" s="6">
+        <v>0.12890625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C23">
+      <c r="C25" s="6">
         <v>46</v>
       </c>
-      <c r="D23">
+      <c r="D25" s="6">
         <v>203</v>
       </c>
-      <c r="E23">
+      <c r="E25" s="6">
         <v>216</v>
       </c>
-      <c r="F23">
+      <c r="F25" s="6">
         <v>47</v>
       </c>
-      <c r="G23">
+      <c r="G25" s="6">
         <v>0.17557251908396901</v>
       </c>
-      <c r="H23">
+      <c r="H25" s="6">
         <v>0.184738955823293</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="I25" s="6">
+        <v>0.181640625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C24">
+      <c r="C26" s="6">
         <v>24</v>
       </c>
-      <c r="D24">
+      <c r="D26" s="6">
         <v>225</v>
       </c>
-      <c r="E24">
+      <c r="E26" s="6">
         <v>244</v>
       </c>
-      <c r="F24">
+      <c r="F26" s="6">
         <v>19</v>
       </c>
-      <c r="G24">
+      <c r="G26" s="6">
         <v>8.9552238805970102E-2</v>
       </c>
-      <c r="H24">
+      <c r="H26" s="6">
         <v>9.6385542168674704E-2</v>
+      </c>
+      <c r="I26" s="6">
+        <v>8.3984375E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="6">
+        <v>27</v>
+      </c>
+      <c r="D27" s="6">
+        <v>222</v>
+      </c>
+      <c r="E27" s="6">
+        <v>244</v>
+      </c>
+      <c r="F27" s="6">
+        <v>19</v>
+      </c>
+      <c r="G27" s="6">
+        <v>9.9630996309963096E-2</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.108433734939759</v>
+      </c>
+      <c r="I27" s="6">
+        <v>8.984375E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="6">
+        <v>17</v>
+      </c>
+      <c r="D28" s="6">
+        <v>232</v>
+      </c>
+      <c r="E28" s="6">
+        <v>245</v>
+      </c>
+      <c r="F28" s="6">
+        <v>18</v>
+      </c>
+      <c r="G28" s="6">
+        <v>6.4885496183206104E-2</v>
+      </c>
+      <c r="H28" s="6">
+        <v>6.82730923694779E-2</v>
+      </c>
+      <c r="I28" s="6">
+        <v>6.8359375E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>0</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="17">
+        <v>24</v>
+      </c>
+      <c r="D39" s="17">
+        <v>42</v>
+      </c>
+      <c r="E39" s="17">
+        <v>36</v>
+      </c>
+      <c r="F39" s="17">
+        <v>29</v>
+      </c>
+      <c r="G39" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="H39" s="17">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="I39" s="17">
+        <v>0.40845070422535201</v>
+      </c>
+      <c r="J39" s="17">
+        <v>0.40458015267175601</v>
+      </c>
+      <c r="K39" s="17">
+        <v>0.19047619047619099</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="9">
+        <v>31</v>
+      </c>
+      <c r="D40" s="9">
+        <v>47</v>
+      </c>
+      <c r="E40" s="9">
+        <v>57</v>
+      </c>
+      <c r="F40" s="9">
+        <v>33</v>
+      </c>
+      <c r="G40" s="9">
+        <v>0.35227272727272702</v>
+      </c>
+      <c r="H40" s="9">
+        <v>0.39743589743589702</v>
+      </c>
+      <c r="I40" s="22">
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="J40" s="9">
+        <v>0.38095238095238099</v>
+      </c>
+      <c r="K40" s="9">
+        <v>0.186746987951807</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="9">
+        <v>31</v>
+      </c>
+      <c r="D41" s="9">
+        <v>79</v>
+      </c>
+      <c r="E41" s="9">
+        <v>65</v>
+      </c>
+      <c r="F41" s="9">
+        <v>33</v>
+      </c>
+      <c r="G41" s="9">
+        <v>0.32291666666666702</v>
+      </c>
+      <c r="H41" s="9">
+        <v>0.28181818181818202</v>
+      </c>
+      <c r="I41" s="9">
+        <v>0.29464285714285698</v>
+      </c>
+      <c r="J41" s="9">
+        <v>0.30769230769230799</v>
+      </c>
+      <c r="K41" s="9">
+        <v>0.15048543689320401</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="9">
+        <v>27</v>
+      </c>
+      <c r="D42" s="9">
+        <v>56</v>
+      </c>
+      <c r="E42" s="9">
+        <v>0</v>
+      </c>
+      <c r="F42" s="9">
+        <v>33</v>
+      </c>
+      <c r="G42" s="9">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9">
+        <v>0.32530120481927699</v>
+      </c>
+      <c r="I42" s="9">
+        <v>0.37078651685393299</v>
+      </c>
+      <c r="J42" s="22">
+        <v>0.51724137931034497</v>
+      </c>
+      <c r="K42" s="22">
+        <v>0.24545454545454501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="9"/>
+      <c r="B43" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="14">
+        <v>24</v>
+      </c>
+      <c r="D43" s="14">
+        <v>31</v>
+      </c>
+      <c r="E43" s="14">
+        <v>49</v>
+      </c>
+      <c r="F43" s="14">
+        <v>16</v>
+      </c>
+      <c r="G43" s="14">
+        <v>0.32876712328767099</v>
+      </c>
+      <c r="H43" s="14">
+        <v>0.43636363636363601</v>
+      </c>
+      <c r="I43" s="14">
+        <v>0.340425531914894</v>
+      </c>
+      <c r="J43" s="14">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="K43" s="15">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="9"/>
+      <c r="B44" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="17">
+        <v>24</v>
+      </c>
+      <c r="D44" s="17">
+        <v>23</v>
+      </c>
+      <c r="E44" s="17">
+        <v>41</v>
+      </c>
+      <c r="F44" s="17">
+        <v>16</v>
+      </c>
+      <c r="G44" s="17">
+        <v>0.36923076923076897</v>
+      </c>
+      <c r="H44" s="17">
+        <v>0.51063829787234005</v>
+      </c>
+      <c r="I44" s="17">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J44" s="17">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="K44" s="18">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="9"/>
+      <c r="B45" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="17">
+        <v>24</v>
+      </c>
+      <c r="D45" s="17">
+        <v>23</v>
+      </c>
+      <c r="E45" s="17">
+        <v>41</v>
+      </c>
+      <c r="F45" s="17">
+        <v>16</v>
+      </c>
+      <c r="G45" s="17">
+        <v>0.36923076923076897</v>
+      </c>
+      <c r="H45" s="17">
+        <v>0.51063829787234005</v>
+      </c>
+      <c r="I45" s="17">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J45" s="17">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="K45" s="18">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="9"/>
+      <c r="B46" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="20">
+        <v>18</v>
+      </c>
+      <c r="D46" s="20">
+        <v>23</v>
+      </c>
+      <c r="E46" s="20">
+        <v>28</v>
+      </c>
+      <c r="F46" s="20">
+        <v>16</v>
+      </c>
+      <c r="G46" s="20">
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="H46" s="20">
+        <v>0.439024390243902</v>
+      </c>
+      <c r="I46" s="20">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J46" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="K46" s="21">
+        <v>0.20689655172413801</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="9">
+        <v>24</v>
+      </c>
+      <c r="D49" s="9">
+        <v>23</v>
+      </c>
+      <c r="E49" s="9">
+        <v>41</v>
+      </c>
+      <c r="F49" s="9">
+        <v>16</v>
+      </c>
+      <c r="G49" s="9">
+        <v>0.36923076923076897</v>
+      </c>
+      <c r="H49" s="9">
+        <v>0.51063829787234005</v>
+      </c>
+      <c r="I49" s="9">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J49" s="9">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="K49" s="9">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="9">
+        <v>31</v>
+      </c>
+      <c r="D50" s="9">
+        <v>55</v>
+      </c>
+      <c r="E50" s="9">
+        <v>65</v>
+      </c>
+      <c r="F50" s="9">
+        <v>33</v>
+      </c>
+      <c r="G50" s="9">
+        <v>0.32291666666666702</v>
+      </c>
+      <c r="H50" s="9">
+        <v>0.36046511627907002</v>
+      </c>
+      <c r="I50" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="J50" s="9">
+        <v>0.34782608695652201</v>
+      </c>
+      <c r="K50" s="9">
+        <v>0.17032967032967</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="9">
+        <v>31</v>
+      </c>
+      <c r="D51" s="9">
+        <v>95</v>
+      </c>
+      <c r="E51" s="9">
+        <v>81</v>
+      </c>
+      <c r="F51" s="9">
+        <v>33</v>
+      </c>
+      <c r="G51" s="9">
+        <v>0.27678571428571402</v>
+      </c>
+      <c r="H51" s="9">
+        <v>0.24603174603174599</v>
+      </c>
+      <c r="I51" s="9">
+        <v>0.2578125</v>
+      </c>
+      <c r="J51" s="9">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="K51" s="9">
+        <v>0.130252100840336</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="9">
+        <v>24</v>
+      </c>
+      <c r="D52" s="9">
+        <v>42</v>
+      </c>
+      <c r="E52" s="9">
+        <v>36</v>
+      </c>
+      <c r="F52" s="9">
+        <v>29</v>
+      </c>
+      <c r="G52" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="H52" s="9">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="I52" s="9">
+        <v>0.40845070422535201</v>
+      </c>
+      <c r="J52" s="12">
+        <v>0.40458015267175601</v>
+      </c>
+      <c r="K52" s="9">
+        <v>0.19047619047619099</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="9"/>
+      <c r="B53" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="14">
+        <v>24</v>
+      </c>
+      <c r="D53" s="14">
+        <v>31</v>
+      </c>
+      <c r="E53" s="14">
+        <v>49</v>
+      </c>
+      <c r="F53" s="14">
+        <v>16</v>
+      </c>
+      <c r="G53" s="14">
+        <v>0.32876712328767099</v>
+      </c>
+      <c r="H53" s="14">
+        <v>0.43636363636363601</v>
+      </c>
+      <c r="I53" s="14">
+        <v>0.340425531914894</v>
+      </c>
+      <c r="J53" s="14">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="K53" s="15">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="9"/>
+      <c r="B54" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="17">
+        <v>24</v>
+      </c>
+      <c r="D54" s="17">
+        <v>23</v>
+      </c>
+      <c r="E54" s="17">
+        <v>41</v>
+      </c>
+      <c r="F54" s="17">
+        <v>16</v>
+      </c>
+      <c r="G54" s="17">
+        <v>0.36923076923076897</v>
+      </c>
+      <c r="H54" s="17">
+        <v>0.51063829787234005</v>
+      </c>
+      <c r="I54" s="17">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J54" s="17">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="K54" s="18">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="9"/>
+      <c r="B55" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="17">
+        <v>24</v>
+      </c>
+      <c r="D55" s="17">
+        <v>23</v>
+      </c>
+      <c r="E55" s="17">
+        <v>41</v>
+      </c>
+      <c r="F55" s="17">
+        <v>16</v>
+      </c>
+      <c r="G55" s="17">
+        <v>0.36923076923076897</v>
+      </c>
+      <c r="H55" s="17">
+        <v>0.51063829787234005</v>
+      </c>
+      <c r="I55" s="17">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J55" s="17">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="K55" s="18">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="9"/>
+      <c r="B56" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="20">
+        <v>20</v>
+      </c>
+      <c r="D56" s="20">
+        <v>17</v>
+      </c>
+      <c r="E56" s="20">
+        <v>51</v>
+      </c>
+      <c r="F56" s="20">
+        <v>2</v>
+      </c>
+      <c r="G56" s="20">
+        <v>0.28169014084506999</v>
+      </c>
+      <c r="H56" s="20">
+        <v>0.54054054054054101</v>
+      </c>
+      <c r="I56" s="20">
+        <v>0.105263157894737</v>
+      </c>
+      <c r="J56" s="20">
+        <v>0.24444444444444399</v>
+      </c>
+      <c r="K56" s="21">
+        <v>0.18518518518518501</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K58" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="9">
+        <v>24</v>
+      </c>
+      <c r="D59" s="9">
+        <v>23</v>
+      </c>
+      <c r="E59" s="9">
+        <v>41</v>
+      </c>
+      <c r="F59" s="9">
+        <v>16</v>
+      </c>
+      <c r="G59" s="9">
+        <v>0.36923076923076897</v>
+      </c>
+      <c r="H59" s="9">
+        <v>0.51063829787234005</v>
+      </c>
+      <c r="I59" s="9">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J59" s="9">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="K59" s="9">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="9">
+        <v>31</v>
+      </c>
+      <c r="D60" s="9">
+        <v>55</v>
+      </c>
+      <c r="E60" s="9">
+        <v>65</v>
+      </c>
+      <c r="F60" s="9">
+        <v>33</v>
+      </c>
+      <c r="G60" s="9">
+        <v>0.32291666666666702</v>
+      </c>
+      <c r="H60" s="9">
+        <v>0.36046511627907002</v>
+      </c>
+      <c r="I60" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="J60" s="9">
+        <v>0.34782608695652201</v>
+      </c>
+      <c r="K60" s="9">
+        <v>0.17032967032967</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" s="9">
+        <v>31</v>
+      </c>
+      <c r="D61" s="9">
+        <v>95</v>
+      </c>
+      <c r="E61" s="9">
+        <v>81</v>
+      </c>
+      <c r="F61" s="9">
+        <v>33</v>
+      </c>
+      <c r="G61" s="9">
+        <v>0.27678571428571402</v>
+      </c>
+      <c r="H61" s="9">
+        <v>0.24603174603174599</v>
+      </c>
+      <c r="I61" s="9">
+        <v>0.2578125</v>
+      </c>
+      <c r="J61" s="9">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="K61" s="9">
+        <v>0.130252100840336</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" s="9">
+        <v>24</v>
+      </c>
+      <c r="D62" s="9">
+        <v>42</v>
+      </c>
+      <c r="E62" s="9">
+        <v>36</v>
+      </c>
+      <c r="F62" s="9">
+        <v>29</v>
+      </c>
+      <c r="G62" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="H62" s="9">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="I62" s="9">
+        <v>0.40845070422535201</v>
+      </c>
+      <c r="J62" s="12">
+        <v>0.40458015267175601</v>
+      </c>
+      <c r="K62" s="9">
+        <v>0.19047619047619099</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="9"/>
+      <c r="B63" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="14">
+        <v>24</v>
+      </c>
+      <c r="D63" s="14">
+        <v>31</v>
+      </c>
+      <c r="E63" s="14">
+        <v>49</v>
+      </c>
+      <c r="F63" s="14">
+        <v>16</v>
+      </c>
+      <c r="G63" s="14">
+        <v>0.32876712328767099</v>
+      </c>
+      <c r="H63" s="14">
+        <v>0.43636363636363601</v>
+      </c>
+      <c r="I63" s="14">
+        <v>0.340425531914894</v>
+      </c>
+      <c r="J63" s="14">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="K63" s="15">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="9"/>
+      <c r="B64" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" s="17">
+        <v>24</v>
+      </c>
+      <c r="D64" s="17">
+        <v>23</v>
+      </c>
+      <c r="E64" s="17">
+        <v>41</v>
+      </c>
+      <c r="F64" s="17">
+        <v>16</v>
+      </c>
+      <c r="G64" s="17">
+        <v>0.36923076923076897</v>
+      </c>
+      <c r="H64" s="17">
+        <v>0.51063829787234005</v>
+      </c>
+      <c r="I64" s="17">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J64" s="17">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="K64" s="18">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="9"/>
+      <c r="B65" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C65" s="17">
+        <v>24</v>
+      </c>
+      <c r="D65" s="17">
+        <v>23</v>
+      </c>
+      <c r="E65" s="17">
+        <v>41</v>
+      </c>
+      <c r="F65" s="17">
+        <v>16</v>
+      </c>
+      <c r="G65" s="17">
+        <v>0.36923076923076897</v>
+      </c>
+      <c r="H65" s="17">
+        <v>0.51063829787234005</v>
+      </c>
+      <c r="I65" s="17">
+        <v>0.41025641025641002</v>
+      </c>
+      <c r="J65" s="17">
+        <v>0.38461538461538503</v>
+      </c>
+      <c r="K65" s="18">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="9"/>
+      <c r="B66" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="20">
+        <v>20</v>
+      </c>
+      <c r="D66" s="20">
+        <v>17</v>
+      </c>
+      <c r="E66" s="20">
+        <v>51</v>
+      </c>
+      <c r="F66" s="20">
+        <v>2</v>
+      </c>
+      <c r="G66" s="20">
+        <v>0.28169014084506999</v>
+      </c>
+      <c r="H66" s="20">
+        <v>0.54054054054054101</v>
+      </c>
+      <c r="I66" s="20">
+        <v>0.105263157894737</v>
+      </c>
+      <c r="J66" s="20">
+        <v>0.24444444444444399</v>
+      </c>
+      <c r="K66" s="21">
+        <v>0.18518518518518501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>